<commit_message>
Add functionality for ontogeny definition in a population.
</commit_message>
<xml_diff>
--- a/inst/extdata/examples/TestProject/Parameters/PopulationParameters.xlsx
+++ b/inst/extdata/examples/TestProject/Parameters/PopulationParameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\tests\data\TestProject\Parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\inst\extdata\examples\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4B8C94-13CA-4464-A6AD-FE203ECC14C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8F1CFC-4CE8-4D8C-8B13-C18E8CE8E9C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19103" yWindow="-98" windowWidth="28995" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demographics" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>PopulationName</t>
   </si>
@@ -116,6 +116,12 @@
   </si>
   <si>
     <t>TestPopulation</t>
+  </si>
+  <si>
+    <t>Ontogeny</t>
+  </si>
+  <si>
+    <t>Protein</t>
   </si>
 </sst>
 </file>
@@ -448,30 +454,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.35"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.1171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5859375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.1171875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.41015625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5859375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.87890625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1171875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.41015625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.87890625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.5859375" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="7.87890625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="8.1171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -520,8 +526,14 @@
       <c r="P1" t="s">
         <v>19</v>
       </c>
+      <c r="Q1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R1" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -568,12 +580,12 @@
       <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.35"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.1171875" customWidth="1"/>
+    <col min="2" max="2" width="19.703125" customWidth="1"/>
+    <col min="3" max="3" width="9.29296875" customWidth="1"/>
+    <col min="4" max="4" width="9.703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Add functionality for ontogeny definition in a population. (#462)
* Add functionality for ontogeny definition in a population.

* Update R/utilities-population.R

Co-authored-by: Felix MIL <34234913+Felixmil@users.noreply.github.com>

* Update R/utilities-population.R

Co-authored-by: Felix MIL <34234913+Felixmil@users.noreply.github.com>

* Update R/utilities-population.R

Co-authored-by: Felix MIL <34234913+Felixmil@users.noreply.github.com>

---------

Co-authored-by: Felix MIL <34234913+Felixmil@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/inst/extdata/examples/TestProject/Parameters/PopulationParameters.xlsx
+++ b/inst/extdata/examples/TestProject/Parameters/PopulationParameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\tests\data\TestProject\Parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\inst\extdata\examples\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4B8C94-13CA-4464-A6AD-FE203ECC14C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8F1CFC-4CE8-4D8C-8B13-C18E8CE8E9C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19103" yWindow="-98" windowWidth="28995" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demographics" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>PopulationName</t>
   </si>
@@ -116,6 +116,12 @@
   </si>
   <si>
     <t>TestPopulation</t>
+  </si>
+  <si>
+    <t>Ontogeny</t>
+  </si>
+  <si>
+    <t>Protein</t>
   </si>
 </sst>
 </file>
@@ -448,30 +454,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.35"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.1171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5859375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.1171875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.41015625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5859375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.87890625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1171875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.41015625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.87890625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.5859375" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="7.87890625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="8.1171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -520,8 +526,14 @@
       <c r="P1" t="s">
         <v>19</v>
       </c>
+      <c r="Q1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R1" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -568,12 +580,12 @@
       <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.35"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.1171875" customWidth="1"/>
+    <col min="2" max="2" width="19.703125" customWidth="1"/>
+    <col min="3" max="3" width="9.29296875" customWidth="1"/>
+    <col min="4" max="4" width="9.703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>